<commit_message>
xls sample data upd
</commit_message>
<xml_diff>
--- a/test_data/sample_info.xlsx
+++ b/test_data/sample_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="580" windowWidth="25040" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sample_info.csv" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Sample Basename</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Read1</t>
   </si>
@@ -33,9 +30,6 @@
     <t>Condition</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>testA</t>
   </si>
   <si>
@@ -58,6 +52,9 @@
   </si>
   <si>
     <t>treatment</t>
+  </si>
+  <si>
+    <t>Sample_Basename</t>
   </si>
 </sst>
 </file>
@@ -426,57 +423,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>